<commit_message>
Work on db and name change
</commit_message>
<xml_diff>
--- a/DataSet schema.xlsx
+++ b/DataSet schema.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkoen\documents\GitHub\Printer-Migration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Randell\Documents\GitHub\Printer-Migration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>DataTable</t>
   </si>
@@ -57,24 +57,6 @@
   </si>
   <si>
     <t>Issue</t>
-  </si>
-  <si>
-    <t>Environment.Username</t>
-  </si>
-  <si>
-    <t>bool flag</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>On or Off</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>remove list</t>
   </si>
 </sst>
 </file>
@@ -392,28 +374,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -427,80 +408,65 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J4" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
         <v>2</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>3</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H5" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I6" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J7" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
         <v>2</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>3</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H8" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I9" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
         <v>1</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>